<commit_message>
Atualizando o relatório e a planilha. Criando menu para testar
</commit_message>
<xml_diff>
--- a/planilha_arvores.xlsx
+++ b/planilha_arvores.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9cca01d0ab6cc38/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{3EF87CCF-0759-429C-AA69-1D3093CFD1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="14_{3EF87CCF-0759-429C-AA69-1D3093CFD1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECC0AF15-4CAE-4166-8BC8-18B647389B06}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{30685898-A731-4577-ACEB-6CA723C0FEE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{30685898-A731-4577-ACEB-6CA723C0FEE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Imagens" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="54">
   <si>
     <t>número de elementos</t>
   </si>
@@ -176,6 +177,27 @@
   </si>
   <si>
     <t>0.1</t>
+  </si>
+  <si>
+    <t>Inserir 20000 AVL e Busca</t>
+  </si>
+  <si>
+    <t>Inserir 10000 AVL e Busca</t>
+  </si>
+  <si>
+    <t>Inserir 500 AVL e Busca</t>
+  </si>
+  <si>
+    <t>Inserir 100 AVL e Busca</t>
+  </si>
+  <si>
+    <t>Inserir 1000 Busca e AVL</t>
+  </si>
+  <si>
+    <t>Inserir 1 milhão AVL e Busca</t>
+  </si>
+  <si>
+    <t>Busca AVL e árvore de Busca</t>
   </si>
 </sst>
 </file>
@@ -419,93 +441,93 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -523,6 +545,319 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>553035</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>143319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8755FA3A-B663-3973-5A1C-5D4E14B420ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1238250" y="390525"/>
+          <a:ext cx="4191585" cy="3181794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>486355</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38494</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B0372EA-E30A-63C9-7A7E-F3DC151CE0C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6086475" y="457200"/>
+          <a:ext cx="4153480" cy="2819794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>524452</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>162330</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2FA22AE-857C-3EB3-B4CC-892012657C8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266825" y="4114800"/>
+          <a:ext cx="4134427" cy="2905530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>543511</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>124215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36602A07-A2F7-5345-980A-0ABA5A514324}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="4191000"/>
+          <a:ext cx="4201111" cy="2791215"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>495880</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>143267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE59C283-7E97-004B-0177-EF6FA6CC1EFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10972800" y="571500"/>
+          <a:ext cx="4153480" cy="2810267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>505406</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38504</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EA3E251-A1F2-92FC-0A8D-EEF597675D89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11582400" y="4000500"/>
+          <a:ext cx="4163006" cy="2896004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457766</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>9912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{669A87B0-DC50-D008-D00B-87E1D11D5320}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276350" y="7715250"/>
+          <a:ext cx="4058216" cy="2772162"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -824,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9976E8FA-856D-4461-B3DA-601D2C618969}">
   <dimension ref="E1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,49 +1177,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
     </row>
     <row r="2" spans="5:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" spans="5:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="3" t="s">
         <v>24</v>
       </c>
@@ -903,11 +1238,11 @@
       <c r="H4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="43">
         <v>100</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
       <c r="L4" s="8" t="s">
         <v>30</v>
       </c>
@@ -919,18 +1254,18 @@
       <c r="E5" s="4">
         <v>500</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="35"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="43">
         <v>500</v>
       </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
       <c r="L5" s="8" t="s">
         <v>30</v>
       </c>
@@ -942,18 +1277,18 @@
       <c r="E6" s="8">
         <v>1000</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="37">
+      <c r="I6" s="43">
         <v>1000</v>
       </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
       <c r="L6" s="8" t="s">
         <v>30</v>
       </c>
@@ -965,18 +1300,18 @@
       <c r="E7" s="8">
         <v>10000</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="37">
+      <c r="I7" s="43">
         <v>10000</v>
       </c>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
       <c r="L7" s="8" t="s">
         <v>30</v>
       </c>
@@ -988,18 +1323,18 @@
       <c r="E8" s="8">
         <v>20000</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="43">
         <v>20000</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
       <c r="L8" s="8" t="s">
         <v>30</v>
       </c>
@@ -1011,18 +1346,18 @@
       <c r="E9" s="8">
         <v>100000</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="35"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="37">
+      <c r="I9" s="43">
         <v>100000</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
       <c r="L9" s="8" t="s">
         <v>29</v>
       </c>
@@ -1034,18 +1369,18 @@
       <c r="E10" s="8">
         <v>1000000</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="27">
         <v>1000000</v>
       </c>
-      <c r="J10" s="47"/>
-      <c r="K10" s="46"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
       <c r="L10" s="8" t="s">
         <v>34</v>
       </c>
@@ -1057,18 +1392,18 @@
       <c r="E11" s="8">
         <v>10000000</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="35"/>
+      <c r="G11" s="42"/>
       <c r="H11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="43">
         <v>10000000</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
       <c r="L11" s="8" t="s">
         <v>28</v>
       </c>
@@ -1077,41 +1412,41 @@
       </c>
     </row>
     <row r="14" spans="5:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
     </row>
     <row r="15" spans="5:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
       <c r="H15" s="9"/>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
     </row>
     <row r="16" spans="5:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="52"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="11" t="s">
         <v>35</v>
       </c>
@@ -1121,20 +1456,20 @@
       <c r="J16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="K16" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="L16" s="51"/>
-      <c r="M16" s="52"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="34"/>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E17" s="12">
         <v>20000</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="41"/>
       <c r="H17" s="13" t="s">
         <v>39</v>
       </c>
@@ -1144,112 +1479,112 @@
       <c r="J17" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
+      <c r="L17" s="41"/>
+      <c r="M17" s="41"/>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E18" s="12">
         <v>100000</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="25"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="23" t="s">
         <v>37</v>
       </c>
       <c r="I18" s="14">
         <v>100000</v>
       </c>
-      <c r="J18" s="48" t="s">
+      <c r="J18" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="24" t="s">
+      <c r="K18" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="41"/>
-      <c r="M18" s="25"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="51"/>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E19" s="12">
         <v>1000</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="25"/>
+      <c r="G19" s="51"/>
       <c r="H19" s="23" t="s">
         <v>38</v>
       </c>
       <c r="I19" s="14">
         <v>1000</v>
       </c>
-      <c r="J19" s="48" t="s">
+      <c r="J19" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="L19" s="41"/>
-      <c r="M19" s="25"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="51"/>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E20" s="12">
         <v>500</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="25"/>
+      <c r="G20" s="51"/>
       <c r="H20" s="23" t="s">
         <v>38</v>
       </c>
       <c r="I20" s="14">
         <v>500</v>
       </c>
-      <c r="J20" s="48" t="s">
+      <c r="J20" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="24" t="s">
+      <c r="K20" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="41"/>
-      <c r="M20" s="25"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="51"/>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E21" s="12">
         <v>100</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="25"/>
+      <c r="G21" s="51"/>
       <c r="H21" s="23" t="s">
         <v>40</v>
       </c>
       <c r="I21" s="14">
         <v>100</v>
       </c>
-      <c r="J21" s="48" t="s">
+      <c r="J21" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="24" t="s">
+      <c r="K21" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="41"/>
-      <c r="M21" s="25"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="51"/>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E22" s="12">
         <v>1000000</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="29"/>
+      <c r="G22" s="41"/>
       <c r="H22" s="13" t="s">
         <v>41</v>
       </c>
@@ -1259,48 +1594,48 @@
       <c r="J22" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
     </row>
     <row r="24" spans="5:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
     </row>
     <row r="25" spans="5:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E26" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G26" s="32"/>
+      <c r="G26" s="49"/>
       <c r="H26" s="17" t="s">
         <v>35</v>
       </c>
@@ -1310,54 +1645,54 @@
       <c r="J26" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="32" t="s">
+      <c r="K26" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E27" s="22">
         <v>100000</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="28"/>
+      <c r="G27" s="36"/>
       <c r="H27" s="21" t="s">
         <v>37</v>
       </c>
       <c r="I27" s="22">
         <v>100000</v>
       </c>
-      <c r="J27" s="49" t="s">
+      <c r="J27" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L27" s="42"/>
-      <c r="M27" s="28"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="36"/>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E28" s="22">
         <v>1000000</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="28"/>
+      <c r="G28" s="36"/>
       <c r="H28" s="21" t="s">
         <v>41</v>
       </c>
       <c r="I28" s="22">
         <v>1000000</v>
       </c>
-      <c r="J28" s="49" t="s">
+      <c r="J28" s="25" t="s">
         <v>41</v>
       </c>
       <c r="K28" s="20"/>
-      <c r="L28" s="53" t="s">
+      <c r="L28" s="26" t="s">
         <v>46</v>
       </c>
       <c r="M28" s="21"/>
@@ -1366,10 +1701,10 @@
       <c r="E29" s="18">
         <v>20000</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="26"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="19" t="s">
         <v>45</v>
       </c>
@@ -1379,20 +1714,20 @@
       <c r="J29" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="K29" s="26" t="s">
+      <c r="K29" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E30" s="18">
         <v>10000</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="26"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="19" t="s">
         <v>44</v>
       </c>
@@ -1402,20 +1737,20 @@
       <c r="J30" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="26" t="s">
+      <c r="K30" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E31" s="18">
         <v>1000</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="19" t="s">
         <v>38</v>
       </c>
@@ -1425,20 +1760,20 @@
       <c r="J31" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="26" t="s">
+      <c r="K31" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E32" s="18">
         <v>500</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="G32" s="26"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="19" t="s">
         <v>29</v>
       </c>
@@ -1448,20 +1783,20 @@
       <c r="J32" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="26" t="s">
+      <c r="K32" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
+      <c r="L32" s="46"/>
+      <c r="M32" s="46"/>
     </row>
     <row r="33" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E33" s="18">
         <v>100</v>
       </c>
-      <c r="F33" s="26" t="s">
+      <c r="F33" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G33" s="26"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="19" t="s">
         <v>29</v>
       </c>
@@ -1471,26 +1806,35 @@
       <c r="J33" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="K33" s="26" t="s">
+      <c r="K33" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="E24:M24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="I25:M25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K33:M33"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="I3:K3"/>
@@ -1505,38 +1849,72 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:M17"/>
     <mergeCell ref="E14:M14"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="I15:M15"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="E24:M24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I25:M25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K26:M26"/>
     <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K33:M33"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="K27:M27"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="K19:M19"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="K20:M20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0491798F-ACEA-487C-A925-01BD2EBE1BFF}">
+  <dimension ref="C2:T40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" t="s">
+        <v>50</v>
+      </c>
+      <c r="T21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>